<commit_message>
autoload database library add database configuration add sample data main view add user controller add user model add user example view
</commit_message>
<xml_diff>
--- a/design/PrimaryData_update.xlsx
+++ b/design/PrimaryData_update.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pornjeds\Google Drive\02 Projects-2017\AmselNutra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10740" activeTab="1" xr2:uid="{6547E20A-897D-4394-B176-383795CDDBEB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10740" xr2:uid="{6547E20A-897D-4394-B176-383795CDDBEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -1643,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D1BB04-5804-4AF8-B758-EDC5D454548A}">
   <dimension ref="B1:P86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,7 +1797,7 @@
         <v>380</v>
       </c>
       <c r="P3" s="1" t="str">
-        <f t="shared" ref="P3:P66" si="0">_xlfn.CONCAT("('",B3,"','",C3,"','",D3,"','",E3,"','",F3,"','",G3,"','",H3,"','",M3,"','",J3,"','",L3,"','",N3,"'),")</f>
+        <f>_xlfn.CONCAT("('",B3,"','",C3,"','",D3,"','",E3,"','",F3,"','",G3,"','",H3,"','",M3,"','",J3,"','",L3,"','",N3,"'),")</f>
         <v>('account2','account2','อารยา ','นะเอ็ม','ดา','0','0','1','1','1','0865521395'),</v>
       </c>
     </row>
@@ -1844,7 +1844,7 @@
         <v>339</v>
       </c>
       <c r="P4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B4,"','",C4,"','",D4,"','",E4,"','",F4,"','",G4,"','",H4,"','",M4,"','",J4,"','",L4,"','",N4,"'),")</f>
         <v>('account3','FBCD0FF0529A3DD9B733884B30941297','กัญฐณา ','แพรริ้วทองคำ','กัญ','0','0','1','1','2','092-236-1956'),</v>
       </c>
     </row>
@@ -1891,7 +1891,7 @@
         <v>340</v>
       </c>
       <c r="P5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B5,"','",C5,"','",D5,"','",E5,"','",F5,"','",G5,"','",H5,"','",M5,"','",J5,"','",L5,"','",N5,"'),")</f>
         <v>('account4','201E9991AFE90C65E13B08B53FB695DE','พิเชษฐ์ ','ผุดผ่อง','ก้างปลา','0','0','1','1','1','098-250-1787'),</v>
       </c>
     </row>
@@ -1935,7 +1935,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B6,"','",C6,"','",D6,"','",E6,"','",F6,"','",G6,"','",H6,"','",M6,"','",J6,"','",L6,"','",N6,"'),")</f>
         <v>('admin','salepro','ADMIN','ADMIN','ADMIN','0','1','1','2','3',''),</v>
       </c>
     </row>
@@ -1976,7 +1976,7 @@
         <v>2</v>
       </c>
       <c r="P7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B7,"','",C7,"','",D7,"','",E7,"','",F7,"','",G7,"','",H7,"','",M7,"','",J7,"','",L7,"','",N7,"'),")</f>
         <v>('BK01','BK01','รุ่งทิวา','มะลิหวน','','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -2023,7 +2023,7 @@
         <v>341</v>
       </c>
       <c r="P8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B8,"','",C8,"','",D8,"','",E8,"','",F8,"','",G8,"','",H8,"','",M8,"','",J8,"','",L8,"','",N8,"'),")</f>
         <v>('BK02','27D680007D116166FAE1207F30FE9D99','ปรีดา ','เมืองสุวรรณ','เล็ก','1','0','1','3','4','089-662-4004'),</v>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
         <v>342</v>
       </c>
       <c r="P9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B9,"','",C9,"','",D9,"','",E9,"','",F9,"','",G9,"','",H9,"','",M9,"','",J9,"','",L9,"','",N9,"'),")</f>
         <v>('BK03','A77FB36177A0BFD11A9EA201690DE8C4','ณัฏธพัชร ','กัญจนาพรพัชธิ์','กิ๊ฟ','1','0','1','3','4','092-924-5663'),</v>
       </c>
     </row>
@@ -2117,7 +2117,7 @@
         <v>343</v>
       </c>
       <c r="P10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B10,"','",C10,"','",D10,"','",E10,"','",F10,"','",G10,"','",H10,"','",M10,"','",J10,"','",L10,"','",N10,"'),")</f>
         <v>('BK04','BKK0004','นิตยาพร ','บัวอิ่น','คุณนิด','1','0','1','3','4','080-508-9944'),</v>
       </c>
     </row>
@@ -2164,7 +2164,7 @@
         <v>344</v>
       </c>
       <c r="P11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B11,"','",C11,"','",D11,"','",E11,"','",F11,"','",G11,"','",H11,"','",M11,"','",J11,"','",L11,"','",N11,"'),")</f>
         <v>('BK05','BKK005','วารินทร์ ','วรชิตสกุล','รินทร์','1','0','1','3','4','092-841-6905'),</v>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
         <v>345</v>
       </c>
       <c r="P12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B12,"','",C12,"','",D12,"','",E12,"','",F12,"','",G12,"','",H12,"','",M12,"','",J12,"','",L12,"','",N12,"'),")</f>
         <v>('BK06','2485925F7259659642E1D3A6DC1EDD07','มัณฑนา ','บุตรอินทร์','มีน','1','0','1','3','4','099-126-7988'),</v>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
         <v>346</v>
       </c>
       <c r="P13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B13,"','",C13,"','",D13,"','",E13,"','",F13,"','",G13,"','",H13,"','",M13,"','",J13,"','",L13,"','",N13,"'),")</f>
         <v>('BKK10','s10s10','วรัตถ์เอก','','วรัตถ์เอก','1','0','2','3','4','092-2718547'),</v>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
         <v>347</v>
       </c>
       <c r="P14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B14,"','",C14,"','",D14,"','",E14,"','",F14,"','",G14,"','",H14,"','",M14,"','",J14,"','",L14,"','",N14,"'),")</f>
         <v>('BKK16','s16s16','ชญาดา','','ชญาดา','1','0','1','3','4','095-9469494'),</v>
       </c>
     </row>
@@ -2340,7 +2340,7 @@
         <v>2</v>
       </c>
       <c r="P15" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B15,"','",C15,"','",D15,"','",E15,"','",F15,"','",G15,"','",H15,"','",M15,"','",J15,"','",L15,"','",N15,"'),")</f>
         <v>('BKK17','BKK17','ทัฏชญานันท์','','ทัฏชญานันท์','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -2381,7 +2381,7 @@
         <v>2</v>
       </c>
       <c r="P16" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B16,"','",C16,"','",D16,"','",E16,"','",F16,"','",G16,"','",H16,"','",M16,"','",J16,"','",L16,"','",N16,"'),")</f>
         <v>('BKK19','BKK19','จิราภา','','จิราภา','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -2422,7 +2422,7 @@
         <v>348</v>
       </c>
       <c r="P17" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B17,"','",C17,"','",D17,"','",E17,"','",F17,"','",G17,"','",H17,"','",M17,"','",J17,"','",L17,"','",N17,"'),")</f>
         <v>('BKK2','s2s2','พิชานันท์','','','1','0','2','3','4','092-4490456'),</v>
       </c>
     </row>
@@ -2466,7 +2466,7 @@
         <v>349</v>
       </c>
       <c r="P18" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B18,"','",C18,"','",D18,"','",E18,"','",F18,"','",G18,"','",H18,"','",M18,"','",J18,"','",L18,"','",N18,"'),")</f>
         <v>('BKK20','s20s20','ณัฐญาวรรณ ','','ณัฐญาวรรณ ','1','0','2','3','4','081-9434755'),</v>
       </c>
     </row>
@@ -2507,7 +2507,7 @@
         <v>2</v>
       </c>
       <c r="P19" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B19,"','",C19,"','",D19,"','",E19,"','",F19,"','",G19,"','",H19,"','",M19,"','",J19,"','",L19,"','",N19,"'),")</f>
         <v>('BKK22','BKK22','ภัทรชัย','','ภัทรชัย','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -2548,7 +2548,7 @@
         <v>2</v>
       </c>
       <c r="P20" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B20,"','",C20,"','",D20,"','",E20,"','",F20,"','",G20,"','",H20,"','",M20,"','",J20,"','",L20,"','",N20,"'),")</f>
         <v>('BKK23','BKK23','รักเร่','','รักเร่','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -2589,7 +2589,7 @@
         <v>2</v>
       </c>
       <c r="P21" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B21,"','",C21,"','",D21,"','",E21,"','",F21,"','",G21,"','",H21,"','",M21,"','",J21,"','",L21,"','",N21,"'),")</f>
         <v>('BKK24','BKK24','พัชรี','','พัชรี','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -2630,7 +2630,7 @@
         <v>2</v>
       </c>
       <c r="P22" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B22,"','",C22,"','",D22,"','",E22,"','",F22,"','",G22,"','",H22,"','",M22,"','",J22,"','",L22,"','",N22,"'),")</f>
         <v>('BKK25','BKK25','ภัทรกร','','ภัทรกร','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -2671,7 +2671,7 @@
         <v>2</v>
       </c>
       <c r="P23" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B23,"','",C23,"','",D23,"','",E23,"','",F23,"','",G23,"','",H23,"','",M23,"','",J23,"','",L23,"','",N23,"'),")</f>
         <v>('BKK27','BKK27','ศิริพร','','ศิริพร','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -2712,7 +2712,7 @@
         <v>2</v>
       </c>
       <c r="P24" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B24,"','",C24,"','",D24,"','",E24,"','",F24,"','",G24,"','",H24,"','",M24,"','",J24,"','",L24,"','",N24,"'),")</f>
         <v>('BKK28','BKK28','ภารดี','','ภารดี','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -2753,7 +2753,7 @@
         <v>350</v>
       </c>
       <c r="P25" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B25,"','",C25,"','",D25,"','",E25,"','",F25,"','",G25,"','",H25,"','",M25,"','",J25,"','",L25,"','",N25,"'),")</f>
         <v>('BKK3','s3s3','ณิชาภา','','','1','0','2','3','4','081-7778319'),</v>
       </c>
     </row>
@@ -2794,7 +2794,7 @@
         <v>2</v>
       </c>
       <c r="P26" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B26,"','",C26,"','",D26,"','",E26,"','",F26,"','",G26,"','",H26,"','",M26,"','",J26,"','",L26,"','",N26,"'),")</f>
         <v>('BKK30','s30s30','เนตรนภา','โภคบุตร','','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -2838,7 +2838,7 @@
         <v>351</v>
       </c>
       <c r="P27" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B27,"','",C27,"','",D27,"','",E27,"','",F27,"','",G27,"','",H27,"','",M27,"','",J27,"','",L27,"','",N27,"'),")</f>
         <v>('BKK33','s33s33','ศิรภัส ','','ศิรภัส ','1','0','2','3','4','084-1399987'),</v>
       </c>
     </row>
@@ -2879,7 +2879,7 @@
         <v>2</v>
       </c>
       <c r="P28" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B28,"','",C28,"','",D28,"','",E28,"','",F28,"','",G28,"','",H28,"','",M28,"','",J28,"','",L28,"','",N28,"'),")</f>
         <v>('BKK34','s34s34','ปณิตา','นนทมาตย์','','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -2926,7 +2926,7 @@
         <v>352</v>
       </c>
       <c r="P29" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B29,"','",C29,"','",D29,"','",E29,"','",F29,"','",G29,"','",H29,"','",M29,"','",J29,"','",L29,"','",N29,"'),")</f>
         <v>('BKK36','s36s36','ธนาวัตน์','พสุรัตน์','ธนาวัตน์ พสุรัตน์','1','0','2','3','4','086-5599956'),</v>
       </c>
     </row>
@@ -2973,7 +2973,7 @@
         <v>353</v>
       </c>
       <c r="P30" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B30,"','",C30,"','",D30,"','",E30,"','",F30,"','",G30,"','",H30,"','",M30,"','",J30,"','",L30,"','",N30,"'),")</f>
         <v>('BKK37','F251A225F9B59688DFF9B50F4D0BA273','สมคิด ','วรชิตสกุล','ตี๋','1','0','1','4','5','091-725-8882'),</v>
       </c>
     </row>
@@ -3014,7 +3014,7 @@
         <v>354</v>
       </c>
       <c r="P31" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B31,"','",C31,"','",D31,"','",E31,"','",F31,"','",G31,"','",H31,"','",M31,"','",J31,"','",L31,"','",N31,"'),")</f>
         <v>('BKK4','s4s4','พงศ์ลาภ','','','1','0','2','3','4','081-8020138'),</v>
       </c>
     </row>
@@ -3058,7 +3058,7 @@
         <v>2</v>
       </c>
       <c r="P32" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B32,"','",C32,"','",D32,"','",E32,"','",F32,"','",G32,"','",H32,"','",M32,"','",J32,"','",L32,"','",N32,"'),")</f>
         <v>('BKK9','s9s9','สุรชัย','ภัทรบรรเจิด','สุรชัย ภัทรบรรเจิด','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -3099,7 +3099,7 @@
         <v>2</v>
       </c>
       <c r="P33" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B33,"','",C33,"','",D33,"','",E33,"','",F33,"','",G33,"','",H33,"','",M33,"','",J33,"','",L33,"','",N33,"'),")</f>
         <v>('Cash','83ECF4422F214C3D3175E9AFA39EEADD','Cash','','Cash','1','0','2','5','6',''),</v>
       </c>
     </row>
@@ -3140,7 +3140,7 @@
         <v>2</v>
       </c>
       <c r="P34" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B34,"','",C34,"','",D34,"','",E34,"','",F34,"','",G34,"','",H34,"','",M34,"','",J34,"','",L34,"','",N34,"'),")</f>
         <v>('HEAD','HEAD','HEAD','','HEAD','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -3181,7 +3181,7 @@
         <v>1</v>
       </c>
       <c r="P35" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B35,"','",C35,"','",D35,"','",E35,"','",F35,"','",G35,"','",H35,"','",M35,"','",J35,"','",L35,"','",N35,"'),")</f>
         <v>('Head BK01','5A272472EC12ACF78E98684FFA22CC8E','เขตว่าง ','กรุงเทพ ปริมณฑล','','1','0','1','4','5',''),</v>
       </c>
     </row>
@@ -3222,7 +3222,7 @@
         <v>1</v>
       </c>
       <c r="P36" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B36,"','",C36,"','",D36,"','",E36,"','",F36,"','",G36,"','",H36,"','",M36,"','",J36,"','",L36,"','",N36,"'),")</f>
         <v>('Head BK02','5A272472EC12ACF78E98684FFA22CC8E','เขตว่าง ','กรุงเทพ','','1','0','1','4','5',''),</v>
       </c>
     </row>
@@ -3263,7 +3263,7 @@
         <v>1</v>
       </c>
       <c r="P37" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B37,"','",C37,"','",D37,"','",E37,"','",F37,"','",G37,"','",H37,"','",M37,"','",J37,"','",L37,"','",N37,"'),")</f>
         <v>('Head BK03','5A272472EC12ACF78E98684FFA22CC8E','เขตว่าง ','กรุงเทพ สมุทรปราการ','','1','0','1','4','5',''),</v>
       </c>
     </row>
@@ -3304,7 +3304,7 @@
         <v>1</v>
       </c>
       <c r="P38" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B38,"','",C38,"','",D38,"','",E38,"','",F38,"','",G38,"','",H38,"','",M38,"','",J38,"','",L38,"','",N38,"'),")</f>
         <v>('Head UP01','FC99B490918BDC2C28704782D5B7924E','เขตว่าง ','ภาคเหนือ','','1','0','1','4','5',''),</v>
       </c>
     </row>
@@ -3345,7 +3345,7 @@
         <v>1</v>
       </c>
       <c r="P39" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B39,"','",C39,"','",D39,"','",E39,"','",F39,"','",G39,"','",H39,"','",M39,"','",J39,"','",L39,"','",N39,"'),")</f>
         <v>('Head UP02','FC99B490918BDC2C28704782D5B7924E','เขตว่าง ','ภาคอีสาน','','1','0','1','4','5',''),</v>
       </c>
     </row>
@@ -3386,7 +3386,7 @@
         <v>1</v>
       </c>
       <c r="P40" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B40,"','",C40,"','",D40,"','",E40,"','",F40,"','",G40,"','",H40,"','",M40,"','",J40,"','",L40,"','",N40,"'),")</f>
         <v>('Head UP03','FC99B490918BDC2C28704782D5B7924E','เขตว่าง ','ภาคตะวันออก','','1','0','1','4','5',''),</v>
       </c>
     </row>
@@ -3427,7 +3427,7 @@
         <v>1</v>
       </c>
       <c r="P41" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B41,"','",C41,"','",D41,"','",E41,"','",F41,"','",G41,"','",H41,"','",M41,"','",J41,"','",L41,"','",N41,"'),")</f>
         <v>('Head UP04','FC99B490918BDC2C28704782D5B7924E','เขตว่าง ','ภาคใต้','','1','0','1','4','5',''),</v>
       </c>
     </row>
@@ -3468,7 +3468,7 @@
         <v>1</v>
       </c>
       <c r="P42" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B42,"','",C42,"','",D42,"','",E42,"','",F42,"','",G42,"','",H42,"','",M42,"','",J42,"','",L42,"','",N42,"'),")</f>
         <v>('Head UP05','FC99B490918BDC2C28704782D5B7924E','เขตว่าง ','ภาคกลาง','','1','0','1','4','5',''),</v>
       </c>
     </row>
@@ -3512,7 +3512,7 @@
         <v>1</v>
       </c>
       <c r="P43" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B43,"','",C43,"','",D43,"','",E43,"','",F43,"','",G43,"','",H43,"','",M43,"','",J43,"','",L43,"','",N43,"'),")</f>
         <v>('HEAD ภาคกลาง','E75237078E15E6B8E9BA579A1F02CAF9','เขตว่าง ','ภาคกลาง','เขตว่าง ภาคกลาง','1','0','1','4','5',''),</v>
       </c>
     </row>
@@ -3556,7 +3556,7 @@
         <v>1</v>
       </c>
       <c r="P44" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B44,"','",C44,"','",D44,"','",E44,"','",F44,"','",G44,"','",H44,"','",M44,"','",J44,"','",L44,"','",N44,"'),")</f>
         <v>('HEAD ภาคเหนือ','5EDA47765770E95ADCD07F4A3A399725','เขตว่าง ','ภาคเหนือ','เขตว่าง ภาคเหนือ','1','0','1','4','5',''),</v>
       </c>
     </row>
@@ -3600,7 +3600,7 @@
         <v>1</v>
       </c>
       <c r="P45" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B45,"','",C45,"','",D45,"','",E45,"','",F45,"','",G45,"','",H45,"','",M45,"','",J45,"','",L45,"','",N45,"'),")</f>
         <v>('HEAD ภาคอีสาน','CE63C154291A862D7C986BAC9B59B955','เขตว่าง ','ภาคอีสาน','เขตว่าง ภาคอีสาน','1','0','1','4','5',''),</v>
       </c>
     </row>
@@ -3641,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="P46" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B46,"','",C46,"','",D46,"','",E46,"','",F46,"','",G46,"','",H46,"','",M46,"','",J46,"','",L46,"','",N46,"'),")</f>
         <v>('Internet','C8205C7636E728D448C2774E6A4A944B','Internet','','Internet','1','0','1','6','7',''),</v>
       </c>
     </row>
@@ -3688,7 +3688,7 @@
         <v>381</v>
       </c>
       <c r="P47" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B47,"','",C47,"','",D47,"','",E47,"','",F47,"','",G47,"','",H47,"','",M47,"','",J47,"','",L47,"','",N47,"'),")</f>
         <v>('md1','md1','ธนบดินทร์ ','แซ่ตั้ง','กี๋','0','1','1','7','8','0819162819'),</v>
       </c>
     </row>
@@ -3735,7 +3735,7 @@
         <v>355</v>
       </c>
       <c r="P48" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B48,"','",C48,"','",D48,"','",E48,"','",F48,"','",G48,"','",H48,"','",M48,"','",J48,"','",L48,"','",N48,"'),")</f>
         <v>('md2','527851852AC8EE86F4935CF23BD429D8','สิปปกร ','ถาวรวันชัย','นก','0','0','1','8','9','081-4384377'),</v>
       </c>
     </row>
@@ -3779,7 +3779,7 @@
         <v>1</v>
       </c>
       <c r="P49" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B49,"','",C49,"','",D49,"','",E49,"','",F49,"','",G49,"','",H49,"','",M49,"','",J49,"','",L49,"','",N49,"'),")</f>
         <v>('mkt01','FE64788E3AAFBEF093FA636FA3C8D5E5','ณัฏฐพร ','เรืองฤทธิ์','ตุ้ม','0','0','1','9','10',''),</v>
       </c>
     </row>
@@ -3820,7 +3820,7 @@
         <v>2</v>
       </c>
       <c r="P50" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B50,"','",C50,"','",D50,"','",E50,"','",F50,"','",G50,"','",H50,"','",M50,"','",J50,"','",L50,"','",N50,"'),")</f>
         <v>('OEM1','s1s1','ปรัศนียาภรณ์','บุษปวนิช','','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -3864,7 +3864,7 @@
         <v>2</v>
       </c>
       <c r="P51" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B51,"','",C51,"','",D51,"','",E51,"','",F51,"','",G51,"','",H51,"','",M51,"','",J51,"','",L51,"','",N51,"'),")</f>
         <v>('OEM2','A0E584E036D17F0572CD9AE1A8AFAFE9','วิภาดา ','ซิ้มสกุล','พี','1','0','2','10','11',''),</v>
       </c>
     </row>
@@ -3911,7 +3911,7 @@
         <v>356</v>
       </c>
       <c r="P52" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B52,"','",C52,"','",D52,"','",E52,"','",F52,"','",G52,"','",H52,"','",M52,"','",J52,"','",L52,"','",N52,"'),")</f>
         <v>('OEM3','1046B627A8895A79DB5CA2F24CF13A91','จุฑาพร ','ญาณแก้ว','อ้อม','1','0','1','4','12','095-858-8849'),</v>
       </c>
     </row>
@@ -3958,7 +3958,7 @@
         <v>357</v>
       </c>
       <c r="P53" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B53,"','",C53,"','",D53,"','",E53,"','",F53,"','",G53,"','",H53,"','",M53,"','",J53,"','",L53,"','",N53,"'),")</f>
         <v>('Online01','882A77633FD094A60FDCE785DC547A5D','เจียระไน ','แสนสุริยวงศ์','แป้ง','1','0','1','11','3','092-4136000'),</v>
       </c>
     </row>
@@ -4005,7 +4005,7 @@
         <v>358</v>
       </c>
       <c r="P54" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B54,"','",C54,"','",D54,"','",E54,"','",F54,"','",G54,"','",H54,"','",M54,"','",J54,"','",L54,"','",N54,"'),")</f>
         <v>('pcsp1','88F82302BD2F770C14AEF8154533D8B7','วนิชชา ','ปีกอง','อี๊ฟ','0','0','1','12','13','092-624-5566'),</v>
       </c>
     </row>
@@ -4052,7 +4052,7 @@
         <v>382</v>
       </c>
       <c r="P55" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B55,"','",C55,"','",D55,"','",E55,"','",F55,"','",G55,"','",H55,"','",M55,"','",J55,"','",L55,"','",N55,"'),")</f>
         <v>('saleco1','saleco1','รังสิรส ','ศิลปเจริญ','รส','0','0','1','13','14','0860185109'),</v>
       </c>
     </row>
@@ -4099,7 +4099,7 @@
         <v>383</v>
       </c>
       <c r="P56" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B56,"','",C56,"','",D56,"','",E56,"','",F56,"','",G56,"','",H56,"','",M56,"','",J56,"','",L56,"','",N56,"'),")</f>
         <v>('saleco2','saleco2','พรทิวา ','ไทยสยาม','กระแต','0','0','1','14','15','0820840144'),</v>
       </c>
     </row>
@@ -4146,7 +4146,7 @@
         <v>359</v>
       </c>
       <c r="P57" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B57,"','",C57,"','",D57,"','",E57,"','",F57,"','",G57,"','",H57,"','",M57,"','",J57,"','",L57,"','",N57,"'),")</f>
         <v>('saleco3','32A025E9FC20F658A4B7FE0ECE613180','ฐาปนี ','เพชรชิต','เอิง','0','0','1','13','14','092-282-9670'),</v>
       </c>
     </row>
@@ -4187,7 +4187,7 @@
         <v>2</v>
       </c>
       <c r="P58" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B58,"','",C58,"','",D58,"','",E58,"','",F58,"','",G58,"','",H58,"','",M58,"','",J58,"','",L58,"','",N58,"'),")</f>
         <v>('UP01','UP01','นภัค','วิชญ์วัชร','','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -4234,7 +4234,7 @@
         <v>360</v>
       </c>
       <c r="P59" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B59,"','",C59,"','",D59,"','",E59,"','",F59,"','",G59,"','",H59,"','",M59,"','",J59,"','",L59,"','",N59,"'),")</f>
         <v>('UP02','UP02','นที ','เกียรติคงศักดิ์','นที','1','0','1','3','4','088-500-2521'),</v>
       </c>
     </row>
@@ -4281,7 +4281,7 @@
         <v>361</v>
       </c>
       <c r="P60" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B60,"','",C60,"','",D60,"','",E60,"','",F60,"','",G60,"','",H60,"','",M60,"','",J60,"','",L60,"','",N60,"'),")</f>
         <v>('UP03','UP03','วรัญญา ','เรืององอาจ','คุณแหม่ม','1','0','1','3','4','087-644-5956'),</v>
       </c>
     </row>
@@ -4325,7 +4325,7 @@
         <v>362</v>
       </c>
       <c r="P61" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B61,"','",C61,"','",D61,"','",E61,"','",F61,"','",G61,"','",H61,"','",M61,"','",J61,"','",L61,"','",N61,"'),")</f>
         <v>('UP04','UP04','สิริชัย','เพิ่มสุขารมย์','','1','0','1','3','4','080-016-5786'),</v>
       </c>
     </row>
@@ -4369,7 +4369,7 @@
         <v>1</v>
       </c>
       <c r="P62" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B62,"','",C62,"','",D62,"','",E62,"','",F62,"','",G62,"','",H62,"','",M62,"','",J62,"','",L62,"','",N62,"'),")</f>
         <v>('UP05','UP05','สุพจน์ ','ณรงค์ศักดิ์','สุพจน์','1','0','1','3','4',''),</v>
       </c>
     </row>
@@ -4413,7 +4413,7 @@
         <v>363</v>
       </c>
       <c r="P63" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B63,"','",C63,"','",D63,"','",E63,"','",F63,"','",G63,"','",H63,"','",M63,"','",J63,"','",L63,"','",N63,"'),")</f>
         <v>('UP06','009D226BCDE38BD85FF8165451E0E6C7','พิสารัตน์ ','ขันธอุบล','','1','0','1','3','4','084-406-4564'),</v>
       </c>
     </row>
@@ -4460,7 +4460,7 @@
         <v>364</v>
       </c>
       <c r="P64" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B64,"','",C64,"','",D64,"','",E64,"','",F64,"','",G64,"','",H64,"','",M64,"','",J64,"','",L64,"','",N64,"'),")</f>
         <v>('UP07','075D6E8A19E3970FD1E94FEA8A1091E4','ธนพัฒน์ ','เนื้อนุ่ม','เปิ้ล','1','0','1','4','5','085-150-0056'),</v>
       </c>
     </row>
@@ -4507,7 +4507,7 @@
         <v>365</v>
       </c>
       <c r="P65" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B65,"','",C65,"','",D65,"','",E65,"','",F65,"','",G65,"','",H65,"','",M65,"','",J65,"','",L65,"','",N65,"'),")</f>
         <v>('UP08','D074A8869601B15CD1155593D16CAC15','ภานุรัศมิ์ ','นวลศรี','ต้อย','1','0','1','4','5','080-448-2589'),</v>
       </c>
     </row>
@@ -4554,7 +4554,7 @@
         <v>366</v>
       </c>
       <c r="P66" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("('",B66,"','",C66,"','",D66,"','",E66,"','",F66,"','",G66,"','",H66,"','",M66,"','",J66,"','",L66,"','",N66,"'),")</f>
         <v>('UP09','B90B7662AE19F53AB63C3764343F0BA9','นัยนา ','เพิ่มทองคำ','ตุ๊ก','1','0','1','4','5','081-498-5535'),</v>
       </c>
     </row>
@@ -4601,7 +4601,7 @@
         <v>367</v>
       </c>
       <c r="P67" s="1" t="str">
-        <f t="shared" ref="P67:P86" si="1">_xlfn.CONCAT("('",B67,"','",C67,"','",D67,"','",E67,"','",F67,"','",G67,"','",H67,"','",M67,"','",J67,"','",L67,"','",N67,"'),")</f>
+        <f>_xlfn.CONCAT("('",B67,"','",C67,"','",D67,"','",E67,"','",F67,"','",G67,"','",H67,"','",M67,"','",J67,"','",L67,"','",N67,"'),")</f>
         <v>('UP10','D45FBA59F704C808BF31BF0983811A9A','ไพโรจน์ ','ภาสุขกมล','โรจน์','1','0','1','3','4','084-358-8989'),</v>
       </c>
     </row>
@@ -4648,7 +4648,7 @@
         <v>368</v>
       </c>
       <c r="P68" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B68,"','",C68,"','",D68,"','",E68,"','",F68,"','",G68,"','",H68,"','",M68,"','",J68,"','",L68,"','",N68,"'),")</f>
         <v>('UP11','462ACC2529D8E1FED7DA1375F84432E7','ณัฐพงศ์ ','แสนสุข','ปอนด์','1','0','1','3','4','086-410-1662'),</v>
       </c>
     </row>
@@ -4689,7 +4689,7 @@
         <v>369</v>
       </c>
       <c r="P69" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B69,"','",C69,"','",D69,"','",E69,"','",F69,"','",G69,"','",H69,"','",M69,"','",J69,"','",L69,"','",N69,"'),")</f>
         <v>('UPC11','s11s11','อรอนงค์ ','','','1','0','2','3','4','080-6443770'),</v>
       </c>
     </row>
@@ -4730,7 +4730,7 @@
         <v>370</v>
       </c>
       <c r="P70" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B70,"','",C70,"','",D70,"','",E70,"','",F70,"','",G70,"','",H70,"','",M70,"','",J70,"','",L70,"','",N70,"'),")</f>
         <v>('UPC12','s12s12','อภิรัฐ ','','','1','0','2','3','4','083-6479246'),</v>
       </c>
     </row>
@@ -4774,7 +4774,7 @@
         <v>371</v>
       </c>
       <c r="P71" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B71,"','",C71,"','",D71,"','",E71,"','",F71,"','",G71,"','",H71,"','",M71,"','",J71,"','",L71,"','",N71,"'),")</f>
         <v>('UPC13','s13s13','ณัฐธมนวรรณ ','','ณัฐธมนวรรณ ','1','0','2','3','4','095-5010134'),</v>
       </c>
     </row>
@@ -4815,7 +4815,7 @@
         <v>2</v>
       </c>
       <c r="P72" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B72,"','",C72,"','",D72,"','",E72,"','",F72,"','",G72,"','",H72,"','",M72,"','",J72,"','",L72,"','",N72,"'),")</f>
         <v>('UPC14','s14s14','วนิดา','ศรีกำเหนิด','','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -4856,7 +4856,7 @@
         <v>2</v>
       </c>
       <c r="P73" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B73,"','",C73,"','",D73,"','",E73,"','",F73,"','",G73,"','",H73,"','",M73,"','",J73,"','",L73,"','",N73,"'),")</f>
         <v>('UPC15','s15s15','กฤตติพัฒน์','การบรรจง','','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -4897,7 +4897,7 @@
         <v>2</v>
       </c>
       <c r="P74" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B74,"','",C74,"','",D74,"','",E74,"','",F74,"','",G74,"','",H74,"','",M74,"','",J74,"','",L74,"','",N74,"'),")</f>
         <v>('UPC18','UPC18','ประวิทย์','','ประวิทย์','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -4938,7 +4938,7 @@
         <v>2</v>
       </c>
       <c r="P75" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B75,"','",C75,"','",D75,"','",E75,"','",F75,"','",G75,"','",H75,"','",M75,"','",J75,"','",L75,"','",N75,"'),")</f>
         <v>('UPC25','s25s25','เจริญรัตน์','ผลบุญญารัตน์','','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -4982,7 +4982,7 @@
         <v>372</v>
       </c>
       <c r="P76" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B76,"','",C76,"','",D76,"','",E76,"','",F76,"','",G76,"','",H76,"','",M76,"','",J76,"','",L76,"','",N76,"'),")</f>
         <v>('UPC31','s31s31','ยุวดี','','ยุวดี','1','0','2','3','4','098-0864592'),</v>
       </c>
     </row>
@@ -5029,7 +5029,7 @@
         <v>373</v>
       </c>
       <c r="P77" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B77,"','",C77,"','",D77,"','",E77,"','",F77,"','",G77,"','",H77,"','",M77,"','",J77,"','",L77,"','",N77,"'),")</f>
         <v>('UPC32','s32s32','สถาภรณ์','สาแก้ว','สถาภรณ์ สาแก้ว','1','0','2','3','4','080-6100399'),</v>
       </c>
     </row>
@@ -5070,7 +5070,7 @@
         <v>374</v>
       </c>
       <c r="P78" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B78,"','",C78,"','",D78,"','",E78,"','",F78,"','",G78,"','",H78,"','",M78,"','",J78,"','",L78,"','",N78,"'),")</f>
         <v>('UPC35','s35s35','ศิริศักดิ์','','','1','0','2','3','4','099-4122945'),</v>
       </c>
     </row>
@@ -5111,7 +5111,7 @@
         <v>2</v>
       </c>
       <c r="P79" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B79,"','",C79,"','",D79,"','",E79,"','",F79,"','",G79,"','",H79,"','",M79,"','",J79,"','",L79,"','",N79,"'),")</f>
         <v>('UPC5','s5s5','ฐาปนีย์','ทอสาร','','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -5152,7 +5152,7 @@
         <v>2</v>
       </c>
       <c r="P80" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B80,"','",C80,"','",D80,"','",E80,"','",F80,"','",G80,"','",H80,"','",M80,"','",J80,"','",L80,"','",N80,"'),")</f>
         <v>('UPC6','s6s6','เพ็ญนภา','พรายงาม','','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -5193,7 +5193,7 @@
         <v>2</v>
       </c>
       <c r="P81" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B81,"','",C81,"','",D81,"','",E81,"','",F81,"','",G81,"','",H81,"','",M81,"','",J81,"','",L81,"','",N81,"'),")</f>
         <v>('UPC7','UPC7','กิ่งแก้ว','','กิ่งแก้ว','1','0','2','3','4',''),</v>
       </c>
     </row>
@@ -5240,7 +5240,7 @@
         <v>375</v>
       </c>
       <c r="P82" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B82,"','",C82,"','",D82,"','",E82,"','",F82,"','",G82,"','",H82,"','",M82,"','",J82,"','",L82,"','",N82,"'),")</f>
         <v>('whd03','DA05CF38B89BC0F6F1E25D62E7F15F4A','พรรษา ','บุญเชิญ','เจิน','0','0','1','15','16','087-918-9325'),</v>
       </c>
     </row>
@@ -5287,7 +5287,7 @@
         <v>376</v>
       </c>
       <c r="P83" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B83,"','",C83,"','",D83,"','",E83,"','",F83,"','",G83,"','",H83,"','",M83,"','",J83,"','",L83,"','",N83,"'),")</f>
         <v>('whd04','25C9F810F7ADD431D3ECFB67AA330CF0','ดาวรุ่ง ','บุญตา','นิว','0','0','1','16','17','097-278-0609'),</v>
       </c>
     </row>
@@ -5334,7 +5334,7 @@
         <v>384</v>
       </c>
       <c r="P84" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B84,"','",C84,"','",D84,"','",E84,"','",F84,"','",G84,"','",H84,"','",M84,"','",J84,"','",L84,"','",N84,"'),")</f>
         <v>('whd1','whd1','รัตนพล ','โพธิ์คุ้ม','กอล์ฟ','0','0','1','15','16','0852307433'),</v>
       </c>
     </row>
@@ -5381,7 +5381,7 @@
         <v>377</v>
       </c>
       <c r="P85" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B85,"','",C85,"','",D85,"','",E85,"','",F85,"','",G85,"','",H85,"','",M85,"','",J85,"','",L85,"','",N85,"'),")</f>
         <v>('whd2','whd037','พรทิวา ','เฮงตระกูล','แฟง','0','0','1','15','16','096-743-8654'),</v>
       </c>
     </row>
@@ -5425,7 +5425,7 @@
         <v>1</v>
       </c>
       <c r="P86" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT("('",B86,"','",C86,"','",D86,"','",E86,"','",F86,"','",G86,"','",H86,"','",M86,"','",J86,"','",L86,"','",N86,"'),")</f>
         <v>('ศิริพรรณ บุญพระธรรม','7C07A67A4D77FC1B50C405F978AA506E','ศิริพรรณ ','บุญพระธรรม','โอ๋','0','0','1','12','18',''),</v>
       </c>
     </row>
@@ -5438,7 +5438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E67D85-248B-418E-85DC-F25F6AEB45E3}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -5825,7 +5825,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E20" si="0">_xlfn.CONCAT("('",B3,"'),")</f>
+        <f t="shared" ref="E3:E19" si="0">_xlfn.CONCAT("('",B3,"'),")</f>
         <v>('Account Manager'),</v>
       </c>
     </row>

</xml_diff>